<commit_message>
incluindo novo arquivo de validação
</commit_message>
<xml_diff>
--- a/arquivos/analise_por_colunas/AnaliseCPF&Nome.xlsx
+++ b/arquivos/analise_por_colunas/AnaliseCPF&Nome.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DadosCarga" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="DadosSistema" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Analise" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Analise" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DadosCarga" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DadosSistema" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,61 @@
           <t>Matricula</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Nome</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_Nome</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;DtNasc</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_DtNasc</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Sexo</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_Sexo</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Matricula</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_Matricula</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>chave</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Resultado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -488,6 +543,61 @@
       <c r="E2" t="n">
         <v>70297</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>039.173.221-88Mário Manoel Calebe Moura</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>039.173.221-881954-09-26</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>039.173.221-88M</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>039.173.221-8870297</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>039.173.221-88Mário Manoel Calebe Moura1954-09-26M70297</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -511,6 +621,61 @@
       <c r="E3" t="n">
         <v>69314</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>876.995.634-09Anthony Henrique Costa</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>876.995.634-091992-03-26</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>876.995.634-09M</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>876.995.634-0969314</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>876.995.634-09Anthony Henrique Costa1992-03-26M69314</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -534,6 +699,61 @@
       <c r="E4" t="n">
         <v>61902</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>193.703.911-001945-07-17</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>193.703.911-00F</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>193.703.911-0061902</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves1945-07-17F61902</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -556,6 +776,61 @@
       </c>
       <c r="E5" t="n">
         <v>38045</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>369.960.476-411944-02-05</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>369.960.476-41F</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>369.960.476-4138045</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>369.960.476-41Marina Sophie Marlene da Luz1944-02-05F38045</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -569,7 +844,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,25 +878,20 @@
           <t>Matricula</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>chaveCPF&amp;Nome</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anthony Henrique Costa</t>
+          <t>Mário Manoel Calebe Moura</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>876.995.634-09</t>
+          <t>039.173.221-88</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>33689</v>
+        <v>19993</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -629,27 +899,22 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>69314</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>876.995.634-09Anthony Henrique Costa</t>
-        </is>
+        <v>70297</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mário Manoel Calebe Moura</t>
+          <t>Anthony Henrique Costa</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>039.173.221-88</t>
+          <t>876.995.634-09</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>19993</v>
+        <v>33689</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -657,12 +922,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>70297</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>039.173.221-88Mário Manoel Calebe Moura</t>
-        </is>
+        <v>69314</v>
       </c>
     </row>
     <row r="4">
@@ -687,11 +947,6 @@
       <c r="E4" t="n">
         <v>61902</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -714,11 +969,6 @@
       </c>
       <c r="E5" t="n">
         <v>38045</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -732,7 +982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -768,33 +1018,43 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ComparaCPF</t>
+          <t>chaveCPF&amp;Nome</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>chaveCPF&amp;Nome</t>
+          <t>chaveCPF&amp;DtNasc</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ComparaCPF_Nome</t>
+          <t>chaveCPF&amp;Sexo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Matricula</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>chave</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mário Manoel Calebe Moura</t>
+          <t>Anthony Henrique Costa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>039.173.221-88</t>
+          <t>876.995.634-09</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>19993</v>
+        <v>33689</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -802,37 +1062,47 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>70297</v>
+        <v>69314</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>876.995.634-09Anthony Henrique Costa</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>039.173.221-88Mário Manoel Calebe Moura</t>
+          <t>876.995.634-091992-03-26</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>876.995.634-09M</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>876.995.634-0969314</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>876.995.634-09Anthony Henrique Costa1992-03-26M69314</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anthony Henrique Costa</t>
+          <t>Mário Manoel Calebe Moura</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>876.995.634-09</t>
+          <t>039.173.221-88</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>33689</v>
+        <v>19993</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -840,21 +1110,31 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>69314</v>
+        <v>70297</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>039.173.221-88Mário Manoel Calebe Moura</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>876.995.634-09Anthony Henrique Costa</t>
+          <t>039.173.221-881954-09-26</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>039.173.221-88M</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>039.173.221-8870297</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>039.173.221-88Mário Manoel Calebe Moura1954-09-26M70297</t>
         </is>
       </c>
     </row>
@@ -882,17 +1162,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
+          <t>193.703.911-001945-07-17</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>193.703.911-00F</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>193.703.911-0061902</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves1945-07-17F61902</t>
         </is>
       </c>
     </row>
@@ -920,17 +1210,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
+          <t>369.960.476-411944-02-05</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>369.960.476-41F</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>369.960.476-4138045</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>369.960.476-41Marina Sophie Marlene da Luz1944-02-05F38045</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Separado o código de exportação da análise
</commit_message>
<xml_diff>
--- a/arquivos/analise_por_colunas/AnaliseCPF&Nome.xlsx
+++ b/arquivos/analise_por_colunas/AnaliseCPF&Nome.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DadosCarga" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="DadosSistema" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Analise" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Analise" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DadosCarga" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DadosSistema" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,61 @@
           <t>Matricula</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Nome</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_Nome</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;DtNasc</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_DtNasc</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Sexo</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_Sexo</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Matricula</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ComparaCPF_Matricula</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>chave</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Resultado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -488,6 +543,61 @@
       <c r="E2" t="n">
         <v>70297</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>039.173.221-88Mário Manoel Calebe Moura</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>039.173.221-881954-09-26</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>039.173.221-88M</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>039.173.221-8870297</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>039.173.221-88Mário Manoel Calebe Moura1954-09-26M70297</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -511,6 +621,61 @@
       <c r="E3" t="n">
         <v>69314</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>876.995.634-09Anthony Henrique Costa</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>876.995.634-091992-03-26</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>876.995.634-09M</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>876.995.634-0969314</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>876.995.634-09Anthony Henrique Costa1992-03-26M69314</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -534,6 +699,61 @@
       <c r="E4" t="n">
         <v>61902</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>193.703.911-001945-07-17</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>193.703.911-00F</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>193.703.911-0061902</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves1945-07-17F61902</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -556,6 +776,61 @@
       </c>
       <c r="E5" t="n">
         <v>38045</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>369.960.476-411944-02-05</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>369.960.476-41F</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>369.960.476-4138045</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>369.960.476-41Marina Sophie Marlene da Luz1944-02-05F38045</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Localizado</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -569,7 +844,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,25 +878,20 @@
           <t>Matricula</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>chaveCPF&amp;Nome</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anthony Henrique Costa</t>
+          <t>Mário Manoel Calebe Moura</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>876.995.634-09</t>
+          <t>039.173.221-88</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>33689</v>
+        <v>19993</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -629,27 +899,22 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>69314</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>876.995.634-09Anthony Henrique Costa</t>
-        </is>
+        <v>70297</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mário Manoel Calebe Moura</t>
+          <t>Anthony Henrique Costa</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>039.173.221-88</t>
+          <t>876.995.634-09</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>19993</v>
+        <v>33689</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -657,12 +922,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>70297</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>039.173.221-88Mário Manoel Calebe Moura</t>
-        </is>
+        <v>69314</v>
       </c>
     </row>
     <row r="4">
@@ -687,11 +947,6 @@
       <c r="E4" t="n">
         <v>61902</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -714,11 +969,6 @@
       </c>
       <c r="E5" t="n">
         <v>38045</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -732,7 +982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -768,33 +1018,43 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ComparaCPF</t>
+          <t>chaveCPF&amp;Nome</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>chaveCPF&amp;Nome</t>
+          <t>chaveCPF&amp;DtNasc</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ComparaCPF_Nome</t>
+          <t>chaveCPF&amp;Sexo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>chaveCPF&amp;Matricula</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>chave</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mário Manoel Calebe Moura</t>
+          <t>Anthony Henrique Costa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>039.173.221-88</t>
+          <t>876.995.634-09</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>19993</v>
+        <v>33689</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -802,37 +1062,47 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>70297</v>
+        <v>69314</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>876.995.634-09Anthony Henrique Costa</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>039.173.221-88Mário Manoel Calebe Moura</t>
+          <t>876.995.634-091992-03-26</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>876.995.634-09M</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>876.995.634-0969314</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>876.995.634-09Anthony Henrique Costa1992-03-26M69314</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anthony Henrique Costa</t>
+          <t>Mário Manoel Calebe Moura</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>876.995.634-09</t>
+          <t>039.173.221-88</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>33689</v>
+        <v>19993</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -840,21 +1110,31 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>69314</v>
+        <v>70297</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>039.173.221-88Mário Manoel Calebe Moura</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>876.995.634-09Anthony Henrique Costa</t>
+          <t>039.173.221-881954-09-26</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>039.173.221-88M</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>039.173.221-8870297</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>039.173.221-88Mário Manoel Calebe Moura1954-09-26M70297</t>
         </is>
       </c>
     </row>
@@ -882,17 +1162,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves</t>
+          <t>193.703.911-001945-07-17</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>193.703.911-00F</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>193.703.911-0061902</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>193.703.911-00Yasmin Eliane Agatha Gonçalves1945-07-17F61902</t>
         </is>
       </c>
     </row>
@@ -920,17 +1210,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>369.960.476-41Marina Sophie Marlene da Luz</t>
+          <t>369.960.476-411944-02-05</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Localizado</t>
+          <t>369.960.476-41F</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>369.960.476-4138045</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>369.960.476-41Marina Sophie Marlene da Luz1944-02-05F38045</t>
         </is>
       </c>
     </row>

</xml_diff>